<commit_message>
my new Commited code
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -12,18 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Product Name</t>
   </si>
   <si>
     <t>Product Price</t>
-  </si>
-  <si>
-    <t>Hydrate &amp; Glow Skin Kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 54.00</t>
   </si>
   <si>
     <t>Apple iPhone 13 (128GB) DarkRed</t>
@@ -32,10 +26,16 @@
     <t xml:space="preserve"> 800.00</t>
   </si>
   <si>
-    <t>Skin Balance Kit</t>
+    <t>Perfect Skin Kit</t>
   </si>
   <si>
-    <t xml:space="preserve"> 65.00</t>
+    <t xml:space="preserve"> 99.00</t>
+  </si>
+  <si>
+    <t>Sleep &amp; Renew Super Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56.00</t>
   </si>
   <si>
     <t>MIRACLE &amp; HYDRAWEAR KIT</t>
@@ -44,37 +44,19 @@
     <t xml:space="preserve"> 59.00</t>
   </si>
   <si>
-    <t>Sleep &amp; Renew Super Serum</t>
+    <t>Clear Skin Kit</t>
   </si>
   <si>
-    <t xml:space="preserve"> 56.00</t>
-  </si>
-  <si>
-    <t>Perfect 10 Serum</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 19.99</t>
-  </si>
-  <si>
-    <t>Perfect Skin Kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 99.00</t>
-  </si>
-  <si>
-    <t>Flawless Matte Foundation linen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 32.00</t>
-  </si>
-  <si>
-    <t>Clear Skin Kit</t>
+    <t xml:space="preserve"> 65.00</t>
   </si>
   <si>
     <t>Miracle Serum</t>
   </si>
   <si>
     <t xml:space="preserve"> 38.00</t>
+  </si>
+  <si>
+    <t>Skin Balance Kit</t>
   </si>
 </sst>
 </file>
@@ -119,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -167,58 +149,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>